<commit_message>
Fixing an issue related to the balancing portfolio treeview visualization
- Fixing an issue related to the balancing portfolio treeview
- Updating the indexer lib spreadsheet data
</commit_message>
<xml_diff>
--- a/indexer_lib/data/CDI.xlsx
+++ b/indexer_lib/data/CDI.xlsx
@@ -409,7 +409,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O23"/>
+  <dimension ref="A1:O24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -465,43 +465,10 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="B2" s="2">
-        <v>0.14949999999999999</v>
-      </c>
-      <c r="C2" s="2">
-        <v>0.13450000000000001</v>
-      </c>
-      <c r="D2" s="2">
-        <v>0.2011</v>
-      </c>
-      <c r="E2" s="2">
-        <v>0.20780000000000001</v>
-      </c>
-      <c r="F2" s="2">
-        <v>0.27029999999999998</v>
-      </c>
-      <c r="G2" s="2">
-        <v>0.30780000000000002</v>
-      </c>
-      <c r="H2" s="2">
-        <v>0.35560000000000003</v>
-      </c>
-      <c r="I2" s="2">
-        <v>0.4279</v>
-      </c>
-      <c r="J2" s="2">
-        <v>0.44190000000000002</v>
-      </c>
-      <c r="K2" s="2">
-        <v>0.48599999999999999</v>
-      </c>
-      <c r="L2" s="2">
-        <v>0.58679999999999999</v>
-      </c>
-      <c r="M2" s="2">
-        <v>0.77</v>
+        <v>0.73229999999999995</v>
       </c>
       <c r="O2" t="s">
         <v>14</v>
@@ -509,862 +476,903 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="B3" s="2">
-        <v>0.37659999999999999</v>
+        <v>0.14949999999999999</v>
       </c>
       <c r="C3" s="2">
-        <v>0.29370000000000002</v>
+        <v>0.13450000000000001</v>
       </c>
       <c r="D3" s="2">
-        <v>0.33839999999999998</v>
+        <v>0.2011</v>
       </c>
       <c r="E3" s="2">
-        <v>0.28489999999999999</v>
+        <v>0.20780000000000001</v>
       </c>
       <c r="F3" s="2">
-        <v>0.23580000000000001</v>
+        <v>0.27029999999999998</v>
       </c>
       <c r="G3" s="2">
-        <v>0.21229999999999999</v>
+        <v>0.30780000000000002</v>
       </c>
       <c r="H3" s="2">
-        <v>0.1943</v>
+        <v>0.35560000000000003</v>
       </c>
       <c r="I3" s="2">
-        <v>0.15989999999999999</v>
+        <v>0.4279</v>
       </c>
       <c r="J3" s="2">
-        <v>0.157</v>
+        <v>0.44190000000000002</v>
       </c>
       <c r="K3" s="2">
-        <v>0.157</v>
+        <v>0.48599999999999999</v>
       </c>
       <c r="L3" s="2">
-        <v>0.14949999999999999</v>
+        <v>0.58679999999999999</v>
       </c>
       <c r="M3" s="2">
-        <v>0.16450000000000001</v>
+        <v>0.76910000000000001</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="B4" s="2">
-        <v>0.54300000000000004</v>
+        <v>0.37659999999999999</v>
       </c>
       <c r="C4" s="2">
-        <v>0.49349999999999999</v>
+        <v>0.29370000000000002</v>
       </c>
       <c r="D4" s="2">
-        <v>0.46879999999999999</v>
+        <v>0.33839999999999998</v>
       </c>
       <c r="E4" s="2">
-        <v>0.51819999999999999</v>
+        <v>0.28489999999999999</v>
       </c>
       <c r="F4" s="2">
-        <v>0.54300000000000004</v>
+        <v>0.23580000000000001</v>
       </c>
       <c r="G4" s="2">
-        <v>0.46879999999999999</v>
+        <v>0.21229999999999999</v>
       </c>
       <c r="H4" s="2">
-        <v>0.56779999999999997</v>
+        <v>0.1943</v>
       </c>
       <c r="I4" s="2">
-        <v>0.50170000000000003</v>
+        <v>0.15989999999999999</v>
       </c>
       <c r="J4" s="2">
-        <v>0.46379999999999999</v>
+        <v>0.157</v>
       </c>
       <c r="K4" s="2">
-        <v>0.4793</v>
+        <v>0.157</v>
       </c>
       <c r="L4" s="2">
-        <v>0.38040000000000002</v>
+        <v>0.14949999999999999</v>
       </c>
       <c r="M4" s="2">
-        <v>0.37469999999999998</v>
+        <v>0.16450000000000001</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="B5" s="2">
-        <v>0.58330000000000004</v>
+        <v>0.54300000000000004</v>
       </c>
       <c r="C5" s="2">
-        <v>0.46489999999999998</v>
+        <v>0.49349999999999999</v>
       </c>
       <c r="D5" s="2">
-        <v>0.53149999999999997</v>
+        <v>0.46879999999999999</v>
       </c>
       <c r="E5" s="2">
-        <v>0.51749999999999996</v>
+        <v>0.51819999999999999</v>
       </c>
       <c r="F5" s="2">
-        <v>0.51749999999999996</v>
+        <v>0.54300000000000004</v>
       </c>
       <c r="G5" s="2">
-        <v>0.51749999999999996</v>
+        <v>0.46879999999999999</v>
       </c>
       <c r="H5" s="2">
-        <v>0.54220000000000002</v>
+        <v>0.56779999999999997</v>
       </c>
       <c r="I5" s="2">
-        <v>0.56689999999999996</v>
+        <v>0.50170000000000003</v>
       </c>
       <c r="J5" s="2">
-        <v>0.46810000000000002</v>
+        <v>0.46379999999999999</v>
       </c>
       <c r="K5" s="2">
-        <v>0.54300000000000004</v>
+        <v>0.4793</v>
       </c>
       <c r="L5" s="2">
-        <v>0.49349999999999999</v>
+        <v>0.38040000000000002</v>
       </c>
       <c r="M5" s="2">
-        <v>0.49349999999999999</v>
+        <v>0.37469999999999998</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="B6" s="2">
-        <v>1.0846</v>
+        <v>0.58330000000000004</v>
       </c>
       <c r="C6" s="2">
-        <v>0.86380000000000001</v>
+        <v>0.46489999999999998</v>
       </c>
       <c r="D6" s="2">
-        <v>1.0504</v>
+        <v>0.53149999999999997</v>
       </c>
       <c r="E6" s="2">
-        <v>0.78520000000000001</v>
+        <v>0.51749999999999996</v>
       </c>
       <c r="F6" s="2">
-        <v>0.92549999999999999</v>
+        <v>0.51749999999999996</v>
       </c>
       <c r="G6" s="2">
-        <v>0.80810000000000004</v>
+        <v>0.51749999999999996</v>
       </c>
       <c r="H6" s="2">
-        <v>0.79710000000000003</v>
+        <v>0.54220000000000002</v>
       </c>
       <c r="I6" s="2">
-        <v>0.8014</v>
+        <v>0.56689999999999996</v>
       </c>
       <c r="J6" s="2">
-        <v>0.63770000000000004</v>
+        <v>0.46810000000000002</v>
       </c>
       <c r="K6" s="2">
-        <v>0.6431</v>
+        <v>0.54300000000000004</v>
       </c>
       <c r="L6" s="2">
-        <v>0.56740000000000002</v>
+        <v>0.49349999999999999</v>
       </c>
       <c r="M6" s="2">
-        <v>0.53759999999999997</v>
+        <v>0.49349999999999999</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="B7" s="2">
-        <v>1.0548999999999999</v>
+        <v>1.0846</v>
       </c>
       <c r="C7" s="2">
-        <v>1.0014000000000001</v>
+        <v>0.86380000000000001</v>
       </c>
       <c r="D7" s="2">
-        <v>1.1605000000000001</v>
+        <v>1.0504</v>
       </c>
       <c r="E7" s="2">
-        <v>1.0544</v>
+        <v>0.78520000000000001</v>
       </c>
       <c r="F7" s="2">
-        <v>1.1073999999999999</v>
+        <v>0.92549999999999999</v>
       </c>
       <c r="G7" s="2">
-        <v>1.1605000000000001</v>
+        <v>0.80810000000000004</v>
       </c>
       <c r="H7" s="2">
-        <v>1.1073999999999999</v>
+        <v>0.79710000000000003</v>
       </c>
       <c r="I7" s="2">
-        <v>1.2135</v>
+        <v>0.8014</v>
       </c>
       <c r="J7" s="2">
-        <v>1.1073999999999999</v>
+        <v>0.63770000000000004</v>
       </c>
       <c r="K7" s="2">
-        <v>1.0474000000000001</v>
+        <v>0.6431</v>
       </c>
       <c r="L7" s="2">
-        <v>1.0367999999999999</v>
+        <v>0.56740000000000002</v>
       </c>
       <c r="M7" s="2">
-        <v>1.1216999999999999</v>
+        <v>0.53759999999999997</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="B8" s="2">
-        <v>0.92930000000000001</v>
+        <v>1.0548999999999999</v>
       </c>
       <c r="C8" s="2">
-        <v>0.81850000000000001</v>
+        <v>1.0014000000000001</v>
       </c>
       <c r="D8" s="2">
-        <v>1.0361</v>
+        <v>1.1605000000000001</v>
       </c>
       <c r="E8" s="2">
-        <v>0.94820000000000004</v>
+        <v>1.0544</v>
       </c>
       <c r="F8" s="2">
-        <v>0.98380000000000001</v>
+        <v>1.1073999999999999</v>
       </c>
       <c r="G8" s="2">
-        <v>1.0658000000000001</v>
+        <v>1.1605000000000001</v>
       </c>
       <c r="H8" s="2">
-        <v>1.1773</v>
+        <v>1.1073999999999999</v>
       </c>
       <c r="I8" s="2">
-        <v>1.1073999999999999</v>
+        <v>1.2135</v>
       </c>
       <c r="J8" s="2">
         <v>1.1073999999999999</v>
       </c>
       <c r="K8" s="2">
-        <v>1.1076999999999999</v>
+        <v>1.0474000000000001</v>
       </c>
       <c r="L8" s="2">
-        <v>1.0550999999999999</v>
+        <v>1.0367999999999999</v>
       </c>
       <c r="M8" s="2">
-        <v>1.1613</v>
+        <v>1.1216999999999999</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>2014</v>
+        <v>2015</v>
       </c>
       <c r="B9" s="2">
-        <v>0.8397</v>
+        <v>0.92930000000000001</v>
       </c>
       <c r="C9" s="2">
-        <v>0.78259999999999996</v>
+        <v>0.81850000000000001</v>
       </c>
       <c r="D9" s="2">
-        <v>0.75990000000000002</v>
+        <v>1.0361</v>
       </c>
       <c r="E9" s="2">
-        <v>0.81540000000000001</v>
+        <v>0.94820000000000004</v>
       </c>
       <c r="F9" s="2">
-        <v>0.85819999999999996</v>
+        <v>0.98380000000000001</v>
       </c>
       <c r="G9" s="2">
-        <v>0.81740000000000002</v>
+        <v>1.0658000000000001</v>
       </c>
       <c r="H9" s="2">
-        <v>0.94040000000000001</v>
+        <v>1.1773</v>
       </c>
       <c r="I9" s="2">
-        <v>0.85950000000000004</v>
+        <v>1.1073999999999999</v>
       </c>
       <c r="J9" s="2">
-        <v>0.90049999999999997</v>
+        <v>1.1073999999999999</v>
       </c>
       <c r="K9" s="2">
-        <v>0.94479999999999997</v>
+        <v>1.1076999999999999</v>
       </c>
       <c r="L9" s="2">
-        <v>0.83779999999999999</v>
+        <v>1.0550999999999999</v>
       </c>
       <c r="M9" s="2">
-        <v>0.95579999999999998</v>
+        <v>1.1613</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>2013</v>
+        <v>2014</v>
       </c>
       <c r="B10" s="2">
-        <v>0.58660000000000001</v>
+        <v>0.8397</v>
       </c>
       <c r="C10" s="2">
-        <v>0.48149999999999998</v>
+        <v>0.78259999999999996</v>
       </c>
       <c r="D10" s="2">
-        <v>0.53769999999999996</v>
+        <v>0.75990000000000002</v>
       </c>
       <c r="E10" s="2">
-        <v>0.6008</v>
+        <v>0.81540000000000001</v>
       </c>
       <c r="F10" s="2">
-        <v>0.58479999999999999</v>
+        <v>0.85819999999999996</v>
       </c>
       <c r="G10" s="2">
-        <v>0.59189999999999998</v>
+        <v>0.81740000000000002</v>
       </c>
       <c r="H10" s="2">
-        <v>0.7087</v>
+        <v>0.94040000000000001</v>
       </c>
       <c r="I10" s="2">
-        <v>0.69569999999999999</v>
+        <v>0.85950000000000004</v>
       </c>
       <c r="J10" s="2">
-        <v>0.69910000000000005</v>
+        <v>0.90049999999999997</v>
       </c>
       <c r="K10" s="2">
-        <v>0.80330000000000001</v>
+        <v>0.94479999999999997</v>
       </c>
       <c r="L10" s="2">
-        <v>0.71050000000000002</v>
+        <v>0.83779999999999999</v>
       </c>
       <c r="M10" s="2">
-        <v>0.78029999999999999</v>
+        <v>0.95579999999999998</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>2012</v>
+        <v>2013</v>
       </c>
       <c r="B11" s="2">
-        <v>0.88529999999999998</v>
+        <v>0.58660000000000001</v>
       </c>
       <c r="C11" s="2">
-        <v>0.74150000000000005</v>
+        <v>0.48149999999999998</v>
       </c>
       <c r="D11" s="2">
-        <v>0.80830000000000002</v>
+        <v>0.53769999999999996</v>
       </c>
       <c r="E11" s="2">
-        <v>0.69989999999999997</v>
+        <v>0.6008</v>
       </c>
       <c r="F11" s="2">
-        <v>0.73240000000000005</v>
+        <v>0.58479999999999999</v>
       </c>
       <c r="G11" s="2">
-        <v>0.63849999999999996</v>
+        <v>0.59189999999999998</v>
       </c>
       <c r="H11" s="2">
-        <v>0.6754</v>
+        <v>0.7087</v>
       </c>
       <c r="I11" s="2">
-        <v>0.6865</v>
+        <v>0.69569999999999999</v>
       </c>
       <c r="J11" s="2">
-        <v>0.53710000000000002</v>
+        <v>0.69910000000000005</v>
       </c>
       <c r="K11" s="2">
-        <v>0.60719999999999996</v>
+        <v>0.80330000000000001</v>
       </c>
       <c r="L11" s="2">
-        <v>0.5444</v>
+        <v>0.71050000000000002</v>
       </c>
       <c r="M11" s="2">
-        <v>0.53420000000000001</v>
+        <v>0.78029999999999999</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="B12" s="2">
-        <v>0.86060000000000003</v>
+        <v>0.88529999999999998</v>
       </c>
       <c r="C12" s="2">
-        <v>0.84240000000000004</v>
+        <v>0.74150000000000005</v>
       </c>
       <c r="D12" s="2">
-        <v>0.91879999999999995</v>
+        <v>0.80830000000000002</v>
       </c>
       <c r="E12" s="2">
-        <v>0.83879999999999999</v>
+        <v>0.69989999999999997</v>
       </c>
       <c r="F12" s="2">
-        <v>0.98519999999999996</v>
+        <v>0.73240000000000005</v>
       </c>
       <c r="G12" s="2">
-        <v>0.9526</v>
+        <v>0.63849999999999996</v>
       </c>
       <c r="H12" s="2">
-        <v>0.96650000000000003</v>
+        <v>0.6754</v>
       </c>
       <c r="I12" s="2">
-        <v>1.0723</v>
+        <v>0.6865</v>
       </c>
       <c r="J12" s="2">
-        <v>0.93969999999999998</v>
+        <v>0.53710000000000002</v>
       </c>
       <c r="K12" s="2">
-        <v>0.88070000000000004</v>
+        <v>0.60719999999999996</v>
       </c>
       <c r="L12" s="2">
-        <v>0.85860000000000003</v>
+        <v>0.5444</v>
       </c>
       <c r="M12" s="2">
-        <v>0.90459999999999996</v>
+        <v>0.53420000000000001</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>2010</v>
+        <v>2011</v>
       </c>
       <c r="B13" s="2">
-        <v>0.65820000000000001</v>
+        <v>0.86060000000000003</v>
       </c>
       <c r="C13" s="2">
-        <v>0.59250000000000003</v>
+        <v>0.84240000000000004</v>
       </c>
       <c r="D13" s="2">
-        <v>0.75690000000000002</v>
+        <v>0.91879999999999995</v>
       </c>
       <c r="E13" s="2">
-        <v>0.66390000000000005</v>
+        <v>0.83879999999999999</v>
       </c>
       <c r="F13" s="2">
-        <v>0.75</v>
+        <v>0.98519999999999996</v>
       </c>
       <c r="G13" s="2">
-        <v>0.79079999999999995</v>
+        <v>0.9526</v>
       </c>
       <c r="H13" s="2">
-        <v>0.85919999999999996</v>
+        <v>0.96650000000000003</v>
       </c>
       <c r="I13" s="2">
-        <v>0.88629999999999998</v>
+        <v>1.0723</v>
       </c>
       <c r="J13" s="2">
-        <v>0.84450000000000003</v>
+        <v>0.93969999999999998</v>
       </c>
       <c r="K13" s="2">
-        <v>0.80559999999999998</v>
+        <v>0.88070000000000004</v>
       </c>
       <c r="L13" s="2">
-        <v>0.80559999999999998</v>
+        <v>0.85860000000000003</v>
       </c>
       <c r="M13" s="2">
-        <v>0.92710000000000004</v>
+        <v>0.90459999999999996</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>2009</v>
+        <v>2010</v>
       </c>
       <c r="B14" s="2">
-        <v>1.0427</v>
+        <v>0.65820000000000001</v>
       </c>
       <c r="C14" s="2">
-        <v>0.85270000000000001</v>
+        <v>0.59250000000000003</v>
       </c>
       <c r="D14" s="2">
-        <v>0.96650000000000003</v>
+        <v>0.75690000000000002</v>
       </c>
       <c r="E14" s="2">
-        <v>0.83560000000000001</v>
+        <v>0.66390000000000005</v>
       </c>
       <c r="F14" s="2">
-        <v>0.76639999999999997</v>
+        <v>0.75</v>
       </c>
       <c r="G14" s="2">
-        <v>0.75139999999999996</v>
+        <v>0.79079999999999995</v>
       </c>
       <c r="H14" s="2">
-        <v>0.78400000000000003</v>
+        <v>0.85919999999999996</v>
       </c>
       <c r="I14" s="2">
-        <v>0.69140000000000001</v>
+        <v>0.88629999999999998</v>
       </c>
       <c r="J14" s="2">
-        <v>0.6915</v>
+        <v>0.84450000000000003</v>
       </c>
       <c r="K14" s="2">
-        <v>0.69120000000000004</v>
+        <v>0.80559999999999998</v>
       </c>
       <c r="L14" s="2">
-        <v>0.65900000000000003</v>
+        <v>0.80559999999999998</v>
       </c>
       <c r="M14" s="2">
-        <v>0.7238</v>
+        <v>0.92710000000000004</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>2008</v>
+        <v>2009</v>
       </c>
       <c r="B15" s="2">
-        <v>0.92159999999999997</v>
+        <v>1.0427</v>
       </c>
       <c r="C15" s="2">
-        <v>0.79479999999999995</v>
+        <v>0.85270000000000001</v>
       </c>
       <c r="D15" s="2">
-        <v>0.83830000000000005</v>
+        <v>0.96650000000000003</v>
       </c>
       <c r="E15" s="2">
-        <v>0.89800000000000002</v>
+        <v>0.83560000000000001</v>
       </c>
       <c r="F15" s="2">
-        <v>0.871</v>
+        <v>0.76639999999999997</v>
       </c>
       <c r="G15" s="2">
-        <v>0.94820000000000004</v>
+        <v>0.75139999999999996</v>
       </c>
       <c r="H15" s="2">
-        <v>1.0640000000000001</v>
+        <v>0.78400000000000003</v>
       </c>
       <c r="I15" s="2">
-        <v>1.0127999999999999</v>
+        <v>0.69140000000000001</v>
       </c>
       <c r="J15" s="2">
-        <v>1.0983000000000001</v>
+        <v>0.6915</v>
       </c>
       <c r="K15" s="2">
-        <v>1.1738999999999999</v>
+        <v>0.69120000000000004</v>
       </c>
       <c r="L15" s="2">
-        <v>0.996</v>
+        <v>0.65900000000000003</v>
       </c>
       <c r="M15" s="2">
-        <v>1.111</v>
+        <v>0.7238</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>2007</v>
+        <v>2008</v>
       </c>
       <c r="B16" s="2">
-        <v>1.08</v>
+        <v>0.92159999999999997</v>
       </c>
       <c r="C16" s="2">
-        <v>0.87</v>
+        <v>0.79479999999999995</v>
       </c>
       <c r="D16" s="2">
-        <v>1.05</v>
+        <v>0.83830000000000005</v>
       </c>
       <c r="E16" s="2">
-        <v>0.94</v>
+        <v>0.89800000000000002</v>
       </c>
       <c r="F16" s="2">
-        <v>1.02</v>
+        <v>0.871</v>
       </c>
       <c r="G16" s="2">
-        <v>0.9</v>
+        <v>0.94820000000000004</v>
       </c>
       <c r="H16" s="2">
-        <v>0.97</v>
+        <v>1.0640000000000001</v>
       </c>
       <c r="I16" s="2">
-        <v>0.99</v>
+        <v>1.0127999999999999</v>
       </c>
       <c r="J16" s="2">
-        <v>0.8</v>
+        <v>1.0983000000000001</v>
       </c>
       <c r="K16" s="2">
-        <v>0.92</v>
+        <v>1.1738999999999999</v>
       </c>
       <c r="L16" s="2">
-        <v>0.84</v>
+        <v>0.996</v>
       </c>
       <c r="M16" s="2">
-        <v>0.84</v>
+        <v>1.111</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>2006</v>
+        <v>2007</v>
       </c>
       <c r="B17" s="2">
-        <v>1.43</v>
+        <v>1.08</v>
       </c>
       <c r="C17" s="2">
-        <v>1.1399999999999999</v>
+        <v>0.87</v>
       </c>
       <c r="D17" s="2">
-        <v>1.42</v>
+        <v>1.05</v>
       </c>
       <c r="E17" s="2">
-        <v>1.08</v>
+        <v>0.94</v>
       </c>
       <c r="F17" s="2">
-        <v>1.28</v>
+        <v>1.02</v>
       </c>
       <c r="G17" s="2">
-        <v>1.18</v>
+        <v>0.9</v>
       </c>
       <c r="H17" s="2">
-        <v>1.17</v>
+        <v>0.97</v>
       </c>
       <c r="I17" s="2">
-        <v>1.25</v>
+        <v>0.99</v>
       </c>
       <c r="J17" s="2">
-        <v>1.05</v>
+        <v>0.8</v>
       </c>
       <c r="K17" s="2">
-        <v>1.0900000000000001</v>
+        <v>0.92</v>
       </c>
       <c r="L17" s="2">
-        <v>1.02</v>
+        <v>0.84</v>
       </c>
       <c r="M17" s="2">
-        <v>0.98</v>
+        <v>0.84</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>2005</v>
+        <v>2006</v>
       </c>
       <c r="B18" s="2">
-        <v>1.38</v>
+        <v>1.43</v>
       </c>
       <c r="C18" s="2">
-        <v>1.22</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="D18" s="2">
-        <v>1.52</v>
+        <v>1.42</v>
       </c>
       <c r="E18" s="2">
-        <v>1.41</v>
+        <v>1.08</v>
       </c>
       <c r="F18" s="2">
-        <v>1.5</v>
+        <v>1.28</v>
       </c>
       <c r="G18" s="2">
-        <v>1.58</v>
+        <v>1.18</v>
       </c>
       <c r="H18" s="2">
-        <v>1.51</v>
+        <v>1.17</v>
       </c>
       <c r="I18" s="2">
-        <v>1.65</v>
+        <v>1.25</v>
       </c>
       <c r="J18" s="2">
-        <v>1.5</v>
+        <v>1.05</v>
       </c>
       <c r="K18" s="2">
-        <v>1.4</v>
+        <v>1.0900000000000001</v>
       </c>
       <c r="L18" s="2">
-        <v>1.38</v>
+        <v>1.02</v>
       </c>
       <c r="M18" s="2">
-        <v>1.47</v>
+        <v>0.98</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>2004</v>
+        <v>2005</v>
       </c>
       <c r="B19" s="2">
-        <v>1.26</v>
+        <v>1.38</v>
       </c>
       <c r="C19" s="2">
-        <v>1.08</v>
+        <v>1.22</v>
       </c>
       <c r="D19" s="2">
-        <v>1.37</v>
+        <v>1.52</v>
       </c>
       <c r="E19" s="2">
-        <v>1.17</v>
+        <v>1.41</v>
       </c>
       <c r="F19" s="2">
-        <v>1.22</v>
+        <v>1.5</v>
       </c>
       <c r="G19" s="2">
-        <v>1.22</v>
+        <v>1.58</v>
       </c>
       <c r="H19" s="2">
-        <v>1.28</v>
+        <v>1.51</v>
       </c>
       <c r="I19" s="2">
-        <v>1.29</v>
+        <v>1.65</v>
       </c>
       <c r="J19" s="2">
-        <v>1.24</v>
+        <v>1.5</v>
       </c>
       <c r="K19" s="2">
-        <v>1.21</v>
+        <v>1.4</v>
       </c>
       <c r="L19" s="2">
-        <v>1.25</v>
+        <v>1.38</v>
       </c>
       <c r="M19" s="2">
-        <v>1.48</v>
+        <v>1.47</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>2003</v>
+        <v>2004</v>
       </c>
       <c r="B20" s="2">
-        <v>1.97</v>
+        <v>1.26</v>
       </c>
       <c r="C20" s="2">
-        <v>1.83</v>
+        <v>1.08</v>
       </c>
       <c r="D20" s="2">
-        <v>1.77</v>
+        <v>1.37</v>
       </c>
       <c r="E20" s="2">
-        <v>1.87</v>
+        <v>1.17</v>
       </c>
       <c r="F20" s="2">
-        <v>1.96</v>
+        <v>1.22</v>
       </c>
       <c r="G20" s="2">
-        <v>1.85</v>
+        <v>1.22</v>
       </c>
       <c r="H20" s="2">
-        <v>2.08</v>
+        <v>1.28</v>
       </c>
       <c r="I20" s="2">
-        <v>1.76</v>
+        <v>1.29</v>
       </c>
       <c r="J20" s="2">
-        <v>1.67</v>
+        <v>1.24</v>
       </c>
       <c r="K20" s="2">
-        <v>1.63</v>
+        <v>1.21</v>
       </c>
       <c r="L20" s="2">
-        <v>1.34</v>
+        <v>1.25</v>
       </c>
       <c r="M20" s="2">
-        <v>1.37</v>
+        <v>1.48</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>2002</v>
+        <v>2003</v>
       </c>
       <c r="B21" s="2">
-        <v>1.53</v>
+        <v>1.97</v>
       </c>
       <c r="C21" s="2">
-        <v>1.25</v>
+        <v>1.83</v>
       </c>
       <c r="D21" s="2">
+        <v>1.77</v>
+      </c>
+      <c r="E21" s="2">
+        <v>1.87</v>
+      </c>
+      <c r="F21" s="2">
+        <v>1.96</v>
+      </c>
+      <c r="G21" s="2">
+        <v>1.85</v>
+      </c>
+      <c r="H21" s="2">
+        <v>2.08</v>
+      </c>
+      <c r="I21" s="2">
+        <v>1.76</v>
+      </c>
+      <c r="J21" s="2">
+        <v>1.67</v>
+      </c>
+      <c r="K21" s="2">
+        <v>1.63</v>
+      </c>
+      <c r="L21" s="2">
+        <v>1.34</v>
+      </c>
+      <c r="M21" s="2">
         <v>1.37</v>
-      </c>
-      <c r="E21" s="2">
-        <v>1.48</v>
-      </c>
-      <c r="F21" s="2">
-        <v>1.4</v>
-      </c>
-      <c r="G21" s="2">
-        <v>1.31</v>
-      </c>
-      <c r="H21" s="2">
-        <v>1.54</v>
-      </c>
-      <c r="I21" s="2">
-        <v>1.45</v>
-      </c>
-      <c r="J21" s="2">
-        <v>1.38</v>
-      </c>
-      <c r="K21" s="2">
-        <v>1.64</v>
-      </c>
-      <c r="L21" s="2">
-        <v>1.53</v>
-      </c>
-      <c r="M21" s="2">
-        <v>1.73</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>2001</v>
+        <v>2002</v>
       </c>
       <c r="B22" s="2">
-        <v>1.26</v>
+        <v>1.53</v>
       </c>
       <c r="C22" s="2">
-        <v>1.01</v>
+        <v>1.25</v>
       </c>
       <c r="D22" s="2">
-        <v>1.25</v>
+        <v>1.37</v>
       </c>
       <c r="E22" s="2">
-        <v>1.18</v>
+        <v>1.48</v>
       </c>
       <c r="F22" s="2">
-        <v>1.33</v>
+        <v>1.4</v>
       </c>
       <c r="G22" s="2">
-        <v>1.27</v>
+        <v>1.31</v>
       </c>
       <c r="H22" s="2">
-        <v>1.5</v>
+        <v>1.54</v>
       </c>
       <c r="I22" s="2">
-        <v>1.6</v>
+        <v>1.45</v>
       </c>
       <c r="J22" s="2">
-        <v>1.32</v>
+        <v>1.38</v>
       </c>
       <c r="K22" s="2">
-        <v>1.54</v>
+        <v>1.64</v>
       </c>
       <c r="L22" s="2">
-        <v>1.39</v>
+        <v>1.53</v>
       </c>
       <c r="M22" s="2">
-        <v>1.39</v>
+        <v>1.73</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
+        <v>2001</v>
+      </c>
+      <c r="B23" s="2">
+        <v>1.26</v>
+      </c>
+      <c r="C23" s="2">
+        <v>1.01</v>
+      </c>
+      <c r="D23" s="2">
+        <v>1.25</v>
+      </c>
+      <c r="E23" s="2">
+        <v>1.18</v>
+      </c>
+      <c r="F23" s="2">
+        <v>1.33</v>
+      </c>
+      <c r="G23" s="2">
+        <v>1.27</v>
+      </c>
+      <c r="H23" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="I23" s="2">
+        <v>1.6</v>
+      </c>
+      <c r="J23" s="2">
+        <v>1.32</v>
+      </c>
+      <c r="K23" s="2">
+        <v>1.54</v>
+      </c>
+      <c r="L23" s="2">
+        <v>1.39</v>
+      </c>
+      <c r="M23" s="2">
+        <v>1.39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
         <v>2000</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B24" s="2">
         <v>1.44</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C24" s="2">
         <v>1.44</v>
       </c>
-      <c r="D23" s="2">
+      <c r="D24" s="2">
         <v>1.44</v>
       </c>
-      <c r="E23" s="2">
+      <c r="E24" s="2">
         <v>1.28</v>
       </c>
-      <c r="F23" s="2">
+      <c r="F24" s="2">
         <v>1.49</v>
       </c>
-      <c r="G23" s="2">
+      <c r="G24" s="2">
         <v>1.39</v>
       </c>
-      <c r="H23" s="2">
+      <c r="H24" s="2">
         <v>1.3</v>
       </c>
-      <c r="I23" s="2">
+      <c r="I24" s="2">
         <v>1.4</v>
       </c>
-      <c r="J23" s="2">
+      <c r="J24" s="2">
         <v>1.22</v>
       </c>
-      <c r="K23" s="2">
+      <c r="K24" s="2">
         <v>1.28</v>
       </c>
-      <c r="L23" s="2">
+      <c r="L24" s="2">
         <v>1.21</v>
       </c>
-      <c r="M23" s="2">
+      <c r="M24" s="2">
         <v>1.19</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updating the indexer data folder (May/2022)
- Updated the indexer data folder
- Change the column names:
  > From "Rentabilidade-média Contratada" to "Taxa-média Contratada"
  > From "Taxa Contratada" to "Taxa-média Contratada"
- Added some "__init__" files
</commit_message>
<xml_diff>
--- a/indexer_lib/data/CDI.xlsx
+++ b/indexer_lib/data/CDI.xlsx
@@ -58,7 +58,7 @@
     <t>Fonte</t>
   </si>
   <si>
-    <t>https://www.portalbrasil.net/indices_cdi/</t>
+    <t>https://www.valor.srv.br/indices/cdi.php</t>
   </si>
 </sst>
 </file>
@@ -68,10 +68,18 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -94,10 +102,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -105,8 +114,10 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -476,7 +487,10 @@
       <c r="D2" s="2">
         <v>0.92710000000000004</v>
       </c>
-      <c r="O2" t="s">
+      <c r="E2" s="2">
+        <v>0.83430000000000004</v>
+      </c>
+      <c r="O2" s="3" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1383,7 +1397,10 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="O2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updating 'indexer_lib\data' with june/july values
</commit_message>
<xml_diff>
--- a/indexer_lib/data/CDI.xlsx
+++ b/indexer_lib/data/CDI.xlsx
@@ -493,6 +493,12 @@
       <c r="F2" s="2">
         <v>1.0346</v>
       </c>
+      <c r="G2" s="2">
+        <v>1.0153000000000001</v>
+      </c>
+      <c r="H2" s="2">
+        <v>1.0348999999999999</v>
+      </c>
       <c r="O2" s="3" t="s">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
Updating 'indexer_lib\data' folder with the most recent values
</commit_message>
<xml_diff>
--- a/indexer_lib/data/CDI.xlsx
+++ b/indexer_lib/data/CDI.xlsx
@@ -502,6 +502,12 @@
       <c r="I2" s="2">
         <v>1.1694</v>
       </c>
+      <c r="J2" s="2">
+        <v>1.0720000000000001</v>
+      </c>
+      <c r="K2" s="2">
+        <v>1.0206999999999999</v>
+      </c>
       <c r="O2" s="3" t="s">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
Updating Indexer lib data
</commit_message>
<xml_diff>
--- a/indexer_lib/data/CDI.xlsx
+++ b/indexer_lib/data/CDI.xlsx
@@ -420,7 +420,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O24"/>
+  <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -476,950 +476,968 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="B2" s="2">
-        <v>0.73229999999999995</v>
+        <v>1.1233</v>
       </c>
       <c r="C2" s="2">
-        <v>0.755</v>
+        <v>0.91810000000000003</v>
       </c>
       <c r="D2" s="2">
-        <v>0.92710000000000004</v>
-      </c>
-      <c r="E2" s="2">
-        <v>0.83430000000000004</v>
-      </c>
-      <c r="F2" s="2">
-        <v>1.0346</v>
-      </c>
-      <c r="G2" s="2">
-        <v>1.0153000000000001</v>
-      </c>
-      <c r="H2" s="2">
-        <v>1.0348999999999999</v>
-      </c>
-      <c r="I2" s="2">
-        <v>1.1694</v>
-      </c>
-      <c r="J2" s="2">
-        <v>1.0720000000000001</v>
-      </c>
-      <c r="K2" s="2">
-        <v>1.0206999999999999</v>
-      </c>
-      <c r="L2" s="2">
-        <v>1.0206999999999999</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>14</v>
-      </c>
+        <v>1.1747000000000001</v>
+      </c>
+      <c r="O2" s="1"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="B3" s="2">
-        <v>0.14949999999999999</v>
+        <v>0.73229999999999995</v>
       </c>
       <c r="C3" s="2">
-        <v>0.13450000000000001</v>
+        <v>0.755</v>
       </c>
       <c r="D3" s="2">
-        <v>0.2011</v>
+        <v>0.92710000000000004</v>
       </c>
       <c r="E3" s="2">
-        <v>0.20780000000000001</v>
+        <v>0.83430000000000004</v>
       </c>
       <c r="F3" s="2">
-        <v>0.27029999999999998</v>
+        <v>1.0346</v>
       </c>
       <c r="G3" s="2">
-        <v>0.30780000000000002</v>
+        <v>1.0153000000000001</v>
       </c>
       <c r="H3" s="2">
-        <v>0.35560000000000003</v>
+        <v>1.0348999999999999</v>
       </c>
       <c r="I3" s="2">
-        <v>0.4279</v>
+        <v>1.1694</v>
       </c>
       <c r="J3" s="2">
-        <v>0.44190000000000002</v>
+        <v>1.0720000000000001</v>
       </c>
       <c r="K3" s="2">
-        <v>0.48599999999999999</v>
+        <v>1.0206999999999999</v>
       </c>
       <c r="L3" s="2">
-        <v>0.58679999999999999</v>
+        <v>1.0206999999999999</v>
       </c>
       <c r="M3" s="2">
-        <v>0.76910000000000001</v>
+        <v>1.1233</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="B4" s="2">
-        <v>0.37659999999999999</v>
+        <v>0.14949999999999999</v>
       </c>
       <c r="C4" s="2">
-        <v>0.29370000000000002</v>
+        <v>0.13450000000000001</v>
       </c>
       <c r="D4" s="2">
-        <v>0.33839999999999998</v>
+        <v>0.2011</v>
       </c>
       <c r="E4" s="2">
-        <v>0.28489999999999999</v>
+        <v>0.20780000000000001</v>
       </c>
       <c r="F4" s="2">
-        <v>0.23580000000000001</v>
+        <v>0.27029999999999998</v>
       </c>
       <c r="G4" s="2">
-        <v>0.21229999999999999</v>
+        <v>0.30780000000000002</v>
       </c>
       <c r="H4" s="2">
-        <v>0.1943</v>
+        <v>0.35560000000000003</v>
       </c>
       <c r="I4" s="2">
-        <v>0.15989999999999999</v>
+        <v>0.4279</v>
       </c>
       <c r="J4" s="2">
-        <v>0.157</v>
+        <v>0.44190000000000002</v>
       </c>
       <c r="K4" s="2">
-        <v>0.157</v>
+        <v>0.48599999999999999</v>
       </c>
       <c r="L4" s="2">
-        <v>0.14949999999999999</v>
+        <v>0.58679999999999999</v>
       </c>
       <c r="M4" s="2">
-        <v>0.16450000000000001</v>
+        <v>0.76910000000000001</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="B5" s="2">
-        <v>0.54300000000000004</v>
+        <v>0.37659999999999999</v>
       </c>
       <c r="C5" s="2">
-        <v>0.49349999999999999</v>
+        <v>0.29370000000000002</v>
       </c>
       <c r="D5" s="2">
-        <v>0.46879999999999999</v>
+        <v>0.33839999999999998</v>
       </c>
       <c r="E5" s="2">
-        <v>0.51819999999999999</v>
+        <v>0.28489999999999999</v>
       </c>
       <c r="F5" s="2">
-        <v>0.54300000000000004</v>
+        <v>0.23580000000000001</v>
       </c>
       <c r="G5" s="2">
-        <v>0.46879999999999999</v>
+        <v>0.21229999999999999</v>
       </c>
       <c r="H5" s="2">
-        <v>0.56779999999999997</v>
+        <v>0.1943</v>
       </c>
       <c r="I5" s="2">
-        <v>0.50170000000000003</v>
+        <v>0.15989999999999999</v>
       </c>
       <c r="J5" s="2">
-        <v>0.46379999999999999</v>
+        <v>0.157</v>
       </c>
       <c r="K5" s="2">
-        <v>0.4793</v>
+        <v>0.157</v>
       </c>
       <c r="L5" s="2">
-        <v>0.38040000000000002</v>
+        <v>0.14949999999999999</v>
       </c>
       <c r="M5" s="2">
-        <v>0.37469999999999998</v>
+        <v>0.16450000000000001</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="B6" s="2">
-        <v>0.58330000000000004</v>
+        <v>0.54300000000000004</v>
       </c>
       <c r="C6" s="2">
-        <v>0.46489999999999998</v>
+        <v>0.49349999999999999</v>
       </c>
       <c r="D6" s="2">
-        <v>0.53149999999999997</v>
+        <v>0.46879999999999999</v>
       </c>
       <c r="E6" s="2">
-        <v>0.51749999999999996</v>
+        <v>0.51819999999999999</v>
       </c>
       <c r="F6" s="2">
-        <v>0.51749999999999996</v>
+        <v>0.54300000000000004</v>
       </c>
       <c r="G6" s="2">
-        <v>0.51749999999999996</v>
+        <v>0.46879999999999999</v>
       </c>
       <c r="H6" s="2">
-        <v>0.54220000000000002</v>
+        <v>0.56779999999999997</v>
       </c>
       <c r="I6" s="2">
-        <v>0.56689999999999996</v>
+        <v>0.50170000000000003</v>
       </c>
       <c r="J6" s="2">
-        <v>0.46810000000000002</v>
+        <v>0.46379999999999999</v>
       </c>
       <c r="K6" s="2">
-        <v>0.54300000000000004</v>
+        <v>0.4793</v>
       </c>
       <c r="L6" s="2">
-        <v>0.49349999999999999</v>
+        <v>0.38040000000000002</v>
       </c>
       <c r="M6" s="2">
-        <v>0.49349999999999999</v>
+        <v>0.37469999999999998</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="B7" s="2">
-        <v>1.0846</v>
+        <v>0.58330000000000004</v>
       </c>
       <c r="C7" s="2">
-        <v>0.86380000000000001</v>
+        <v>0.46489999999999998</v>
       </c>
       <c r="D7" s="2">
-        <v>1.0504</v>
+        <v>0.53149999999999997</v>
       </c>
       <c r="E7" s="2">
-        <v>0.78520000000000001</v>
+        <v>0.51749999999999996</v>
       </c>
       <c r="F7" s="2">
-        <v>0.92549999999999999</v>
+        <v>0.51749999999999996</v>
       </c>
       <c r="G7" s="2">
-        <v>0.80810000000000004</v>
+        <v>0.51749999999999996</v>
       </c>
       <c r="H7" s="2">
-        <v>0.79710000000000003</v>
+        <v>0.54220000000000002</v>
       </c>
       <c r="I7" s="2">
-        <v>0.8014</v>
+        <v>0.56689999999999996</v>
       </c>
       <c r="J7" s="2">
-        <v>0.63770000000000004</v>
+        <v>0.46810000000000002</v>
       </c>
       <c r="K7" s="2">
-        <v>0.6431</v>
+        <v>0.54300000000000004</v>
       </c>
       <c r="L7" s="2">
-        <v>0.56740000000000002</v>
+        <v>0.49349999999999999</v>
       </c>
       <c r="M7" s="2">
-        <v>0.53759999999999997</v>
+        <v>0.49349999999999999</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="B8" s="2">
-        <v>1.0548999999999999</v>
+        <v>1.0846</v>
       </c>
       <c r="C8" s="2">
-        <v>1.0014000000000001</v>
+        <v>0.86380000000000001</v>
       </c>
       <c r="D8" s="2">
-        <v>1.1605000000000001</v>
+        <v>1.0504</v>
       </c>
       <c r="E8" s="2">
-        <v>1.0544</v>
+        <v>0.78520000000000001</v>
       </c>
       <c r="F8" s="2">
-        <v>1.1073999999999999</v>
+        <v>0.92549999999999999</v>
       </c>
       <c r="G8" s="2">
-        <v>1.1605000000000001</v>
+        <v>0.80810000000000004</v>
       </c>
       <c r="H8" s="2">
-        <v>1.1073999999999999</v>
+        <v>0.79710000000000003</v>
       </c>
       <c r="I8" s="2">
-        <v>1.2135</v>
+        <v>0.8014</v>
       </c>
       <c r="J8" s="2">
-        <v>1.1073999999999999</v>
+        <v>0.63770000000000004</v>
       </c>
       <c r="K8" s="2">
-        <v>1.0474000000000001</v>
+        <v>0.6431</v>
       </c>
       <c r="L8" s="2">
-        <v>1.0367999999999999</v>
+        <v>0.56740000000000002</v>
       </c>
       <c r="M8" s="2">
-        <v>1.1216999999999999</v>
+        <v>0.53759999999999997</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="B9" s="2">
-        <v>0.92930000000000001</v>
+        <v>1.0548999999999999</v>
       </c>
       <c r="C9" s="2">
-        <v>0.81850000000000001</v>
+        <v>1.0014000000000001</v>
       </c>
       <c r="D9" s="2">
-        <v>1.0361</v>
+        <v>1.1605000000000001</v>
       </c>
       <c r="E9" s="2">
-        <v>0.94820000000000004</v>
+        <v>1.0544</v>
       </c>
       <c r="F9" s="2">
-        <v>0.98380000000000001</v>
+        <v>1.1073999999999999</v>
       </c>
       <c r="G9" s="2">
-        <v>1.0658000000000001</v>
+        <v>1.1605000000000001</v>
       </c>
       <c r="H9" s="2">
-        <v>1.1773</v>
+        <v>1.1073999999999999</v>
       </c>
       <c r="I9" s="2">
-        <v>1.1073999999999999</v>
+        <v>1.2135</v>
       </c>
       <c r="J9" s="2">
         <v>1.1073999999999999</v>
       </c>
       <c r="K9" s="2">
-        <v>1.1076999999999999</v>
+        <v>1.0474000000000001</v>
       </c>
       <c r="L9" s="2">
-        <v>1.0550999999999999</v>
+        <v>1.0367999999999999</v>
       </c>
       <c r="M9" s="2">
-        <v>1.1613</v>
+        <v>1.1216999999999999</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>2014</v>
+        <v>2015</v>
       </c>
       <c r="B10" s="2">
-        <v>0.8397</v>
+        <v>0.92930000000000001</v>
       </c>
       <c r="C10" s="2">
-        <v>0.78259999999999996</v>
+        <v>0.81850000000000001</v>
       </c>
       <c r="D10" s="2">
-        <v>0.75990000000000002</v>
+        <v>1.0361</v>
       </c>
       <c r="E10" s="2">
-        <v>0.81540000000000001</v>
+        <v>0.94820000000000004</v>
       </c>
       <c r="F10" s="2">
-        <v>0.85819999999999996</v>
+        <v>0.98380000000000001</v>
       </c>
       <c r="G10" s="2">
-        <v>0.81740000000000002</v>
+        <v>1.0658000000000001</v>
       </c>
       <c r="H10" s="2">
-        <v>0.94040000000000001</v>
+        <v>1.1773</v>
       </c>
       <c r="I10" s="2">
-        <v>0.85950000000000004</v>
+        <v>1.1073999999999999</v>
       </c>
       <c r="J10" s="2">
-        <v>0.90049999999999997</v>
+        <v>1.1073999999999999</v>
       </c>
       <c r="K10" s="2">
-        <v>0.94479999999999997</v>
+        <v>1.1076999999999999</v>
       </c>
       <c r="L10" s="2">
-        <v>0.83779999999999999</v>
+        <v>1.0550999999999999</v>
       </c>
       <c r="M10" s="2">
-        <v>0.95579999999999998</v>
+        <v>1.1613</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>2013</v>
+        <v>2014</v>
       </c>
       <c r="B11" s="2">
-        <v>0.58660000000000001</v>
+        <v>0.8397</v>
       </c>
       <c r="C11" s="2">
-        <v>0.48149999999999998</v>
+        <v>0.78259999999999996</v>
       </c>
       <c r="D11" s="2">
-        <v>0.53769999999999996</v>
+        <v>0.75990000000000002</v>
       </c>
       <c r="E11" s="2">
-        <v>0.6008</v>
+        <v>0.81540000000000001</v>
       </c>
       <c r="F11" s="2">
-        <v>0.58479999999999999</v>
+        <v>0.85819999999999996</v>
       </c>
       <c r="G11" s="2">
-        <v>0.59189999999999998</v>
+        <v>0.81740000000000002</v>
       </c>
       <c r="H11" s="2">
-        <v>0.7087</v>
+        <v>0.94040000000000001</v>
       </c>
       <c r="I11" s="2">
-        <v>0.69569999999999999</v>
+        <v>0.85950000000000004</v>
       </c>
       <c r="J11" s="2">
-        <v>0.69910000000000005</v>
+        <v>0.90049999999999997</v>
       </c>
       <c r="K11" s="2">
-        <v>0.80330000000000001</v>
+        <v>0.94479999999999997</v>
       </c>
       <c r="L11" s="2">
-        <v>0.71050000000000002</v>
+        <v>0.83779999999999999</v>
       </c>
       <c r="M11" s="2">
-        <v>0.78029999999999999</v>
+        <v>0.95579999999999998</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>2012</v>
+        <v>2013</v>
       </c>
       <c r="B12" s="2">
-        <v>0.88529999999999998</v>
+        <v>0.58660000000000001</v>
       </c>
       <c r="C12" s="2">
-        <v>0.74150000000000005</v>
+        <v>0.48149999999999998</v>
       </c>
       <c r="D12" s="2">
-        <v>0.80830000000000002</v>
+        <v>0.53769999999999996</v>
       </c>
       <c r="E12" s="2">
-        <v>0.69989999999999997</v>
+        <v>0.6008</v>
       </c>
       <c r="F12" s="2">
-        <v>0.73240000000000005</v>
+        <v>0.58479999999999999</v>
       </c>
       <c r="G12" s="2">
-        <v>0.63849999999999996</v>
+        <v>0.59189999999999998</v>
       </c>
       <c r="H12" s="2">
-        <v>0.6754</v>
+        <v>0.7087</v>
       </c>
       <c r="I12" s="2">
-        <v>0.6865</v>
+        <v>0.69569999999999999</v>
       </c>
       <c r="J12" s="2">
-        <v>0.53710000000000002</v>
+        <v>0.69910000000000005</v>
       </c>
       <c r="K12" s="2">
-        <v>0.60719999999999996</v>
+        <v>0.80330000000000001</v>
       </c>
       <c r="L12" s="2">
-        <v>0.5444</v>
+        <v>0.71050000000000002</v>
       </c>
       <c r="M12" s="2">
-        <v>0.53420000000000001</v>
+        <v>0.78029999999999999</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="B13" s="2">
-        <v>0.86060000000000003</v>
+        <v>0.88529999999999998</v>
       </c>
       <c r="C13" s="2">
-        <v>0.84240000000000004</v>
+        <v>0.74150000000000005</v>
       </c>
       <c r="D13" s="2">
-        <v>0.91879999999999995</v>
+        <v>0.80830000000000002</v>
       </c>
       <c r="E13" s="2">
-        <v>0.83879999999999999</v>
+        <v>0.69989999999999997</v>
       </c>
       <c r="F13" s="2">
-        <v>0.98519999999999996</v>
+        <v>0.73240000000000005</v>
       </c>
       <c r="G13" s="2">
-        <v>0.9526</v>
+        <v>0.63849999999999996</v>
       </c>
       <c r="H13" s="2">
-        <v>0.96650000000000003</v>
+        <v>0.6754</v>
       </c>
       <c r="I13" s="2">
-        <v>1.0723</v>
+        <v>0.6865</v>
       </c>
       <c r="J13" s="2">
-        <v>0.93969999999999998</v>
+        <v>0.53710000000000002</v>
       </c>
       <c r="K13" s="2">
-        <v>0.88070000000000004</v>
+        <v>0.60719999999999996</v>
       </c>
       <c r="L13" s="2">
-        <v>0.85860000000000003</v>
+        <v>0.5444</v>
       </c>
       <c r="M13" s="2">
-        <v>0.90459999999999996</v>
+        <v>0.53420000000000001</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>2010</v>
+        <v>2011</v>
       </c>
       <c r="B14" s="2">
-        <v>0.65820000000000001</v>
+        <v>0.86060000000000003</v>
       </c>
       <c r="C14" s="2">
-        <v>0.59250000000000003</v>
+        <v>0.84240000000000004</v>
       </c>
       <c r="D14" s="2">
-        <v>0.75690000000000002</v>
+        <v>0.91879999999999995</v>
       </c>
       <c r="E14" s="2">
-        <v>0.66390000000000005</v>
+        <v>0.83879999999999999</v>
       </c>
       <c r="F14" s="2">
-        <v>0.75</v>
+        <v>0.98519999999999996</v>
       </c>
       <c r="G14" s="2">
-        <v>0.79079999999999995</v>
+        <v>0.9526</v>
       </c>
       <c r="H14" s="2">
-        <v>0.85919999999999996</v>
+        <v>0.96650000000000003</v>
       </c>
       <c r="I14" s="2">
-        <v>0.88629999999999998</v>
+        <v>1.0723</v>
       </c>
       <c r="J14" s="2">
-        <v>0.84450000000000003</v>
+        <v>0.93969999999999998</v>
       </c>
       <c r="K14" s="2">
-        <v>0.80559999999999998</v>
+        <v>0.88070000000000004</v>
       </c>
       <c r="L14" s="2">
-        <v>0.80559999999999998</v>
+        <v>0.85860000000000003</v>
       </c>
       <c r="M14" s="2">
-        <v>0.92710000000000004</v>
+        <v>0.90459999999999996</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>2009</v>
+        <v>2010</v>
       </c>
       <c r="B15" s="2">
-        <v>1.0427</v>
+        <v>0.65820000000000001</v>
       </c>
       <c r="C15" s="2">
-        <v>0.85270000000000001</v>
+        <v>0.59250000000000003</v>
       </c>
       <c r="D15" s="2">
-        <v>0.96650000000000003</v>
+        <v>0.75690000000000002</v>
       </c>
       <c r="E15" s="2">
-        <v>0.83560000000000001</v>
+        <v>0.66390000000000005</v>
       </c>
       <c r="F15" s="2">
-        <v>0.76639999999999997</v>
+        <v>0.75</v>
       </c>
       <c r="G15" s="2">
-        <v>0.75139999999999996</v>
+        <v>0.79079999999999995</v>
       </c>
       <c r="H15" s="2">
-        <v>0.78400000000000003</v>
+        <v>0.85919999999999996</v>
       </c>
       <c r="I15" s="2">
-        <v>0.69140000000000001</v>
+        <v>0.88629999999999998</v>
       </c>
       <c r="J15" s="2">
-        <v>0.6915</v>
+        <v>0.84450000000000003</v>
       </c>
       <c r="K15" s="2">
-        <v>0.69120000000000004</v>
+        <v>0.80559999999999998</v>
       </c>
       <c r="L15" s="2">
-        <v>0.65900000000000003</v>
+        <v>0.80559999999999998</v>
       </c>
       <c r="M15" s="2">
-        <v>0.7238</v>
+        <v>0.92710000000000004</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>2008</v>
+        <v>2009</v>
       </c>
       <c r="B16" s="2">
-        <v>0.92159999999999997</v>
+        <v>1.0427</v>
       </c>
       <c r="C16" s="2">
-        <v>0.79479999999999995</v>
+        <v>0.85270000000000001</v>
       </c>
       <c r="D16" s="2">
-        <v>0.83830000000000005</v>
+        <v>0.96650000000000003</v>
       </c>
       <c r="E16" s="2">
-        <v>0.89800000000000002</v>
+        <v>0.83560000000000001</v>
       </c>
       <c r="F16" s="2">
-        <v>0.871</v>
+        <v>0.76639999999999997</v>
       </c>
       <c r="G16" s="2">
-        <v>0.94820000000000004</v>
+        <v>0.75139999999999996</v>
       </c>
       <c r="H16" s="2">
-        <v>1.0640000000000001</v>
+        <v>0.78400000000000003</v>
       </c>
       <c r="I16" s="2">
-        <v>1.0127999999999999</v>
+        <v>0.69140000000000001</v>
       </c>
       <c r="J16" s="2">
-        <v>1.0983000000000001</v>
+        <v>0.6915</v>
       </c>
       <c r="K16" s="2">
-        <v>1.1738999999999999</v>
+        <v>0.69120000000000004</v>
       </c>
       <c r="L16" s="2">
-        <v>0.996</v>
+        <v>0.65900000000000003</v>
       </c>
       <c r="M16" s="2">
-        <v>1.111</v>
+        <v>0.7238</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>2007</v>
+        <v>2008</v>
       </c>
       <c r="B17" s="2">
-        <v>1.08</v>
+        <v>0.92159999999999997</v>
       </c>
       <c r="C17" s="2">
-        <v>0.87</v>
+        <v>0.79479999999999995</v>
       </c>
       <c r="D17" s="2">
-        <v>1.05</v>
+        <v>0.83830000000000005</v>
       </c>
       <c r="E17" s="2">
-        <v>0.94</v>
+        <v>0.89800000000000002</v>
       </c>
       <c r="F17" s="2">
-        <v>1.02</v>
+        <v>0.871</v>
       </c>
       <c r="G17" s="2">
-        <v>0.9</v>
+        <v>0.94820000000000004</v>
       </c>
       <c r="H17" s="2">
-        <v>0.97</v>
+        <v>1.0640000000000001</v>
       </c>
       <c r="I17" s="2">
-        <v>0.99</v>
+        <v>1.0127999999999999</v>
       </c>
       <c r="J17" s="2">
-        <v>0.8</v>
+        <v>1.0983000000000001</v>
       </c>
       <c r="K17" s="2">
-        <v>0.92</v>
+        <v>1.1738999999999999</v>
       </c>
       <c r="L17" s="2">
-        <v>0.84</v>
+        <v>0.996</v>
       </c>
       <c r="M17" s="2">
-        <v>0.84</v>
+        <v>1.111</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>2006</v>
+        <v>2007</v>
       </c>
       <c r="B18" s="2">
-        <v>1.43</v>
+        <v>1.08</v>
       </c>
       <c r="C18" s="2">
-        <v>1.1399999999999999</v>
+        <v>0.87</v>
       </c>
       <c r="D18" s="2">
-        <v>1.42</v>
+        <v>1.05</v>
       </c>
       <c r="E18" s="2">
-        <v>1.08</v>
+        <v>0.94</v>
       </c>
       <c r="F18" s="2">
-        <v>1.28</v>
+        <v>1.02</v>
       </c>
       <c r="G18" s="2">
-        <v>1.18</v>
+        <v>0.9</v>
       </c>
       <c r="H18" s="2">
-        <v>1.17</v>
+        <v>0.97</v>
       </c>
       <c r="I18" s="2">
-        <v>1.25</v>
+        <v>0.99</v>
       </c>
       <c r="J18" s="2">
-        <v>1.05</v>
+        <v>0.8</v>
       </c>
       <c r="K18" s="2">
-        <v>1.0900000000000001</v>
+        <v>0.92</v>
       </c>
       <c r="L18" s="2">
-        <v>1.02</v>
+        <v>0.84</v>
       </c>
       <c r="M18" s="2">
-        <v>0.98</v>
+        <v>0.84</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>2005</v>
+        <v>2006</v>
       </c>
       <c r="B19" s="2">
-        <v>1.38</v>
+        <v>1.43</v>
       </c>
       <c r="C19" s="2">
-        <v>1.22</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="D19" s="2">
-        <v>1.52</v>
+        <v>1.42</v>
       </c>
       <c r="E19" s="2">
-        <v>1.41</v>
+        <v>1.08</v>
       </c>
       <c r="F19" s="2">
-        <v>1.5</v>
+        <v>1.28</v>
       </c>
       <c r="G19" s="2">
-        <v>1.58</v>
+        <v>1.18</v>
       </c>
       <c r="H19" s="2">
-        <v>1.51</v>
+        <v>1.17</v>
       </c>
       <c r="I19" s="2">
-        <v>1.65</v>
+        <v>1.25</v>
       </c>
       <c r="J19" s="2">
-        <v>1.5</v>
+        <v>1.05</v>
       </c>
       <c r="K19" s="2">
-        <v>1.4</v>
+        <v>1.0900000000000001</v>
       </c>
       <c r="L19" s="2">
-        <v>1.38</v>
+        <v>1.02</v>
       </c>
       <c r="M19" s="2">
-        <v>1.47</v>
+        <v>0.98</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>2004</v>
+        <v>2005</v>
       </c>
       <c r="B20" s="2">
-        <v>1.26</v>
+        <v>1.38</v>
       </c>
       <c r="C20" s="2">
-        <v>1.08</v>
+        <v>1.22</v>
       </c>
       <c r="D20" s="2">
-        <v>1.37</v>
+        <v>1.52</v>
       </c>
       <c r="E20" s="2">
-        <v>1.17</v>
+        <v>1.41</v>
       </c>
       <c r="F20" s="2">
-        <v>1.22</v>
+        <v>1.5</v>
       </c>
       <c r="G20" s="2">
-        <v>1.22</v>
+        <v>1.58</v>
       </c>
       <c r="H20" s="2">
-        <v>1.28</v>
+        <v>1.51</v>
       </c>
       <c r="I20" s="2">
-        <v>1.29</v>
+        <v>1.65</v>
       </c>
       <c r="J20" s="2">
-        <v>1.24</v>
+        <v>1.5</v>
       </c>
       <c r="K20" s="2">
-        <v>1.21</v>
+        <v>1.4</v>
       </c>
       <c r="L20" s="2">
-        <v>1.25</v>
+        <v>1.38</v>
       </c>
       <c r="M20" s="2">
-        <v>1.48</v>
+        <v>1.47</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>2003</v>
+        <v>2004</v>
       </c>
       <c r="B21" s="2">
-        <v>1.97</v>
+        <v>1.26</v>
       </c>
       <c r="C21" s="2">
-        <v>1.83</v>
+        <v>1.08</v>
       </c>
       <c r="D21" s="2">
-        <v>1.77</v>
+        <v>1.37</v>
       </c>
       <c r="E21" s="2">
-        <v>1.87</v>
+        <v>1.17</v>
       </c>
       <c r="F21" s="2">
-        <v>1.96</v>
+        <v>1.22</v>
       </c>
       <c r="G21" s="2">
-        <v>1.85</v>
+        <v>1.22</v>
       </c>
       <c r="H21" s="2">
-        <v>2.08</v>
+        <v>1.28</v>
       </c>
       <c r="I21" s="2">
-        <v>1.76</v>
+        <v>1.29</v>
       </c>
       <c r="J21" s="2">
-        <v>1.67</v>
+        <v>1.24</v>
       </c>
       <c r="K21" s="2">
-        <v>1.63</v>
+        <v>1.21</v>
       </c>
       <c r="L21" s="2">
-        <v>1.34</v>
+        <v>1.25</v>
       </c>
       <c r="M21" s="2">
-        <v>1.37</v>
+        <v>1.48</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>2002</v>
+        <v>2003</v>
       </c>
       <c r="B22" s="2">
-        <v>1.53</v>
+        <v>1.97</v>
       </c>
       <c r="C22" s="2">
-        <v>1.25</v>
+        <v>1.83</v>
       </c>
       <c r="D22" s="2">
+        <v>1.77</v>
+      </c>
+      <c r="E22" s="2">
+        <v>1.87</v>
+      </c>
+      <c r="F22" s="2">
+        <v>1.96</v>
+      </c>
+      <c r="G22" s="2">
+        <v>1.85</v>
+      </c>
+      <c r="H22" s="2">
+        <v>2.08</v>
+      </c>
+      <c r="I22" s="2">
+        <v>1.76</v>
+      </c>
+      <c r="J22" s="2">
+        <v>1.67</v>
+      </c>
+      <c r="K22" s="2">
+        <v>1.63</v>
+      </c>
+      <c r="L22" s="2">
+        <v>1.34</v>
+      </c>
+      <c r="M22" s="2">
         <v>1.37</v>
-      </c>
-      <c r="E22" s="2">
-        <v>1.48</v>
-      </c>
-      <c r="F22" s="2">
-        <v>1.4</v>
-      </c>
-      <c r="G22" s="2">
-        <v>1.31</v>
-      </c>
-      <c r="H22" s="2">
-        <v>1.54</v>
-      </c>
-      <c r="I22" s="2">
-        <v>1.45</v>
-      </c>
-      <c r="J22" s="2">
-        <v>1.38</v>
-      </c>
-      <c r="K22" s="2">
-        <v>1.64</v>
-      </c>
-      <c r="L22" s="2">
-        <v>1.53</v>
-      </c>
-      <c r="M22" s="2">
-        <v>1.73</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>2001</v>
+        <v>2002</v>
       </c>
       <c r="B23" s="2">
-        <v>1.26</v>
+        <v>1.53</v>
       </c>
       <c r="C23" s="2">
-        <v>1.01</v>
+        <v>1.25</v>
       </c>
       <c r="D23" s="2">
-        <v>1.25</v>
+        <v>1.37</v>
       </c>
       <c r="E23" s="2">
-        <v>1.18</v>
+        <v>1.48</v>
       </c>
       <c r="F23" s="2">
-        <v>1.33</v>
+        <v>1.4</v>
       </c>
       <c r="G23" s="2">
-        <v>1.27</v>
+        <v>1.31</v>
       </c>
       <c r="H23" s="2">
-        <v>1.5</v>
+        <v>1.54</v>
       </c>
       <c r="I23" s="2">
-        <v>1.6</v>
+        <v>1.45</v>
       </c>
       <c r="J23" s="2">
-        <v>1.32</v>
+        <v>1.38</v>
       </c>
       <c r="K23" s="2">
-        <v>1.54</v>
+        <v>1.64</v>
       </c>
       <c r="L23" s="2">
-        <v>1.39</v>
+        <v>1.53</v>
       </c>
       <c r="M23" s="2">
-        <v>1.39</v>
+        <v>1.73</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
+        <v>2001</v>
+      </c>
+      <c r="B24" s="2">
+        <v>1.26</v>
+      </c>
+      <c r="C24" s="2">
+        <v>1.01</v>
+      </c>
+      <c r="D24" s="2">
+        <v>1.25</v>
+      </c>
+      <c r="E24" s="2">
+        <v>1.18</v>
+      </c>
+      <c r="F24" s="2">
+        <v>1.33</v>
+      </c>
+      <c r="G24" s="2">
+        <v>1.27</v>
+      </c>
+      <c r="H24" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="I24" s="2">
+        <v>1.6</v>
+      </c>
+      <c r="J24" s="2">
+        <v>1.32</v>
+      </c>
+      <c r="K24" s="2">
+        <v>1.54</v>
+      </c>
+      <c r="L24" s="2">
+        <v>1.39</v>
+      </c>
+      <c r="M24" s="2">
+        <v>1.39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
         <v>2000</v>
       </c>
-      <c r="B24" s="2">
+      <c r="B25" s="2">
         <v>1.44</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C25" s="2">
         <v>1.44</v>
       </c>
-      <c r="D24" s="2">
+      <c r="D25" s="2">
         <v>1.44</v>
       </c>
-      <c r="E24" s="2">
+      <c r="E25" s="2">
         <v>1.28</v>
       </c>
-      <c r="F24" s="2">
+      <c r="F25" s="2">
         <v>1.49</v>
       </c>
-      <c r="G24" s="2">
+      <c r="G25" s="2">
         <v>1.39</v>
       </c>
-      <c r="H24" s="2">
+      <c r="H25" s="2">
         <v>1.3</v>
       </c>
-      <c r="I24" s="2">
+      <c r="I25" s="2">
         <v>1.4</v>
       </c>
-      <c r="J24" s="2">
+      <c r="J25" s="2">
         <v>1.22</v>
       </c>
-      <c r="K24" s="2">
+      <c r="K25" s="2">
         <v>1.28</v>
       </c>
-      <c r="L24" s="2">
+      <c r="L25" s="2">
         <v>1.21</v>
       </c>
-      <c r="M24" s="2">
+      <c r="M25" s="2">
         <v>1.19</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="O2" r:id="rId1"/>
+    <hyperlink ref="O3" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
Updating apps in LinksMenu
- Updating indexer lib data
- Removing the 'profitability' menu, since the app became unavailable
- Replacing the 'fixedIncome' link, since the previous app became unavailable
- Adding the link to the 'Economic Indexer' app that I am developing
</commit_message>
<xml_diff>
--- a/indexer_lib/data/CDI.xlsx
+++ b/indexer_lib/data/CDI.xlsx
@@ -487,6 +487,15 @@
       <c r="D2" s="2">
         <v>1.1747000000000001</v>
       </c>
+      <c r="E2" s="2">
+        <v>0.91810000000000003</v>
+      </c>
+      <c r="F2" s="2">
+        <v>1.1233</v>
+      </c>
+      <c r="G2" s="2">
+        <v>1.0720000000000001</v>
+      </c>
       <c r="O2" s="1"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">

</xml_diff>